<commit_message>
Update Plantilla carga datos.xlsx
</commit_message>
<xml_diff>
--- a/Plantilla carga datos/Plantilla carga datos.xlsx
+++ b/Plantilla carga datos/Plantilla carga datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Thinkpad E14\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo Thinkpad E14\Documents\GitHub\Arkad\Plantilla carga datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D1BEA1-B0C8-48B1-A55C-02B6ED18EB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1E80AD-4CD7-4BCF-9624-D8489622F66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CFA501B6-8271-423C-A00F-145B11D41630}"/>
   </bookViews>
@@ -36,30 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>pos</t>
-  </si>
-  <si>
-    <t>pred</t>
-  </si>
-  <si>
-    <t>real</t>
-  </si>
-  <si>
-    <t>acierto</t>
-  </si>
-  <si>
-    <t>cumsum</t>
-  </si>
-  <si>
-    <t>accu</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
   <si>
     <t>Fila 2 y fila 3 se utilizan de ejemplo</t>
+  </si>
+  <si>
+    <t>proba(0)</t>
+  </si>
+  <si>
+    <t>proba(1)</t>
+  </si>
+  <si>
+    <t>toggle_false</t>
+  </si>
+  <si>
+    <t>toggle_true</t>
+  </si>
+  <si>
+    <t>threshold</t>
   </si>
 </sst>
 </file>
@@ -482,11 +479,14 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="32.5546875" customWidth="1"/>
   </cols>
@@ -496,77 +496,65 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="J1" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45047</v>
       </c>
-      <c r="B2">
-        <v>7527</v>
+      <c r="B2" s="3">
+        <v>45047</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.36666666666666659</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E3" si="0">IF(D2&gt;I$2,1,0)</f>
         <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>45047</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45048</v>
       </c>
-      <c r="B3">
-        <v>7528</v>
+      <c r="B3" s="3">
+        <v>45048</v>
       </c>
       <c r="C3">
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="D3">
+        <v>0.48333333333333328</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>45048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>